<commit_message>
Added import on admin
</commit_message>
<xml_diff>
--- a/Test_Schedules_Import.xlsx
+++ b/Test_Schedules_Import.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wavephysics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626809F9-0DE8-4530-ACBE-B66759ED5BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A08B344-F457-428B-AB48-6C5F3292ACB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t>Equipment</t>
   </si>
@@ -83,13 +83,55 @@
   </si>
   <si>
     <t>2024-03-15</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Umer</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Bamberg</t>
+  </si>
+  <si>
+    <t>US 1</t>
+  </si>
+  <si>
+    <t>Erlangen</t>
+  </si>
+  <si>
+    <t>CT Room 102</t>
+  </si>
+  <si>
+    <t>US 2</t>
+  </si>
+  <si>
+    <t>2024-01-16</t>
+  </si>
+  <si>
+    <t>2024-02-16</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>2024-02-02</t>
+  </si>
+  <si>
+    <t>2024-03-02</t>
+  </si>
+  <si>
+    <t>2024-03-16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +144,12 @@
       <sz val="11"/>
       <color rgb="FF2D3234"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -437,89 +485,186 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="22" customWidth="1"/>
+    <col min="3" max="9" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
-        <v>20</v>
+      <c r="E7" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added interval field to excel file
</commit_message>
<xml_diff>
--- a/Test_Schedules_Import.xlsx
+++ b/Test_Schedules_Import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wave\WavePhysics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C463780-7683-4E5A-A807-24193FE591BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558339B1-0783-40A1-8AD0-32622FE4C280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
   <si>
     <t>Equipment</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>Saad</t>
+  </si>
+  <si>
+    <t>Interval</t>
   </si>
 </sst>
 </file>
@@ -488,18 +491,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="9" width="22" customWidth="1"/>
+    <col min="3" max="10" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -519,16 +522,19 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -547,17 +553,20 @@
       <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -576,11 +585,14 @@
       <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="I3" t="s">
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="J3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -596,8 +608,11 @@
       <c r="E4" t="s">
         <v>20</v>
       </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -616,17 +631,20 @@
       <c r="F5" t="s">
         <v>30</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
         <v>31</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>11</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -645,11 +663,14 @@
       <c r="F6" t="s">
         <v>33</v>
       </c>
-      <c r="I6" t="s">
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="J6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -665,8 +686,11 @@
       <c r="E7" t="s">
         <v>34</v>
       </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -685,13 +709,16 @@
       <c r="F8" t="s">
         <v>9</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
         <v>10</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>11</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>